<commit_message>
20210917 update codes from Google Drive. (lastest 20210917) I will comment later.
</commit_message>
<xml_diff>
--- a/admin/output.xlsx
+++ b/admin/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>ทดสอบ</t>
   </si>
@@ -35,22 +35,28 @@
     <t>รหัสวิชา</t>
   </si>
   <si>
+    <t>ชื่อระดับการศึกษา</t>
+  </si>
+  <si>
     <t>ระดับชั้นเรียน</t>
   </si>
   <si>
-    <t>วันพุธ</t>
-  </si>
-  <si>
-    <t>14:00 - 15:00</t>
-  </si>
-  <si>
-    <t>ป.1/1</t>
-  </si>
-  <si>
-    <t>ค 11101</t>
+    <t>วันศุกร์</t>
+  </si>
+  <si>
+    <t>15:00 - 16:00</t>
+  </si>
+  <si>
+    <t>ป.4/2</t>
+  </si>
+  <si>
+    <t>ส 21101</t>
   </si>
   <si>
     <t>ประถมศึกษา</t>
+  </si>
+  <si>
+    <t>ประถมปลาย</t>
   </si>
 </sst>
 </file>
@@ -389,22 +395,23 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8.140625" customWidth="true" style="0"/>
     <col min="2" max="2" width="14.42578125" customWidth="true" style="0"/>
-    <col min="3" max="3" width="12.42578125" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12.7109375" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.140625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="10.7109375" customWidth="true" style="0"/>
+    <col min="4" max="4" width="14.85546875" customWidth="true" style="0"/>
+    <col min="5" max="5" width="16.42578125" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.140625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,10 +419,13 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>2561</v>
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -431,22 +441,28 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>